<commit_message>
update content for personality career
</commit_message>
<xml_diff>
--- a/db/csv/personality_category_majors_and_careers.xlsx
+++ b/db/csv/personality_category_majors_and_careers.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>code</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>career_codes</t>
+  </si>
+  <si>
+    <t>career_mame</t>
   </si>
   <si>
     <t>real001</t>
@@ -91,7 +94,8 @@
 per_maj_096;
 per_maj_097;
 per_maj_098;
-per_maj_050;</t>
+per_maj_050;
+per_maj_115;</t>
   </si>
   <si>
     <t>វិទ្យាសាស្ត្រសត្វ;
@@ -117,7 +121,46 @@
 សេដ្ឋកិច្ចព័ត៌មានវិទ្យា;</t>
   </si>
   <si>
-    <t>car_sci_0001</t>
+    <t>car_sci_0030;
+car_sci_0031;
+car_sci_0010;
+car_sci_0001;
+car_sci_0032;
+car_sci_0033;
+car_sci_0034;
+car_sci_0035;
+car_tec_0001;
+car_tec_0015;
+car_soc_0038;
+car_sci_0036;
+car_sci_0037;
+car_sci_0038;
+car_sci_0039;
+car_sci_0040;
+car_sci_0041;
+car_sci_0042;
+car_soc_0045;</t>
+  </si>
+  <si>
+    <t>អ្នកគ្រប់គ្រងកសិដ្ឋាន;
+រដ្ឋបាលព្រៃឈើ;
+ទន្ដពេទ្យ;
+វិស្វករសំណង់ស៊ីវិល;
+វិស្វករអគ្គិសនី;
+វិស្វករគ្រឿងយន្ដកសិកម្ម;
+វិស្វករមេកានិច;
+វិស្វករកុំព្យូទ័រ;
+ស្ថាបត្យករ;
+ពេទ្យសត្វ;
+បុរាណវិទូ;
+ជាងគំនូរ-ចម្លាក់;
+អ្នកបច្ចេកទេសសេដ្ឋកិច្ចព័ត៌មានវិទ្យា;
+អ្នកបច្ចេកទេសបរិស្ថាន;
+អ្នកបច្ចេកទេសគណិតសាស្ត្រ;
+ភូគព្ភវិទូ;
+អ្នកបើកបរ;
+អ្នកបច្ចេកទេសទីពិសោធន៍;
+មន្ត្រីនគរបាល;</t>
   </si>
   <si>
     <t>inv001</t>
@@ -180,6 +223,48 @@
 ប្រវត្តិវិទ្យា;</t>
   </si>
   <si>
+    <t xml:space="preserve">car_sci_0030;
+car_sci_0031;
+car_sci_0043;
+car_sci_0008;
+car_sci_0044
+car_sci_0001;
+car_sci_0032;
+car_sci_0033;
+car_sci_0034;
+car_sci_0035;
+car_tec_0001;
+car_tec_0015;
+car_soc_0038;
+car_sci_0037;
+car_sci_0038;
+car_sci_0039;
+car_sci_0040;
+car_sci_0042;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">អ្នកគ្រប់គ្រងកសិដ្ឋាន;
+រដ្ឋបាលព្រៃឈើ;
+អ្នកបច្ចេកទេសខាងចំណីអាហារ;
+អ្នកបច្ចេកទេសកសិកម្ម;
+វិស្វករគីមីសាស្ត្រ
+វិស្វករសំណង់ស៊ីវិល;
+វិស្វករអគ្គិសនី;
+វិស្វករគ្រឿងយន្ដកសិកម្ម;
+វិស្វករមេកានិច;
+វិស្វករកុំព្យូទ័រ;
+ស្ថាបត្យករ;
+ពេទ្យសត្វ;
+បុរាណវិទូ;
+អ្នកបច្ចេកទេសសេដ្ឋកិច្ចព័ត៌មានវិទ្យា;
+អ្នកបច្ចេកទេសបរិស្ថាន;
+អ្នកបច្ចេកទេសគណិតសាស្ត្រ;
+ភូគព្ភវិទូ;
+អ្នកបច្ចេកទេសទីពិសោធន៍;
+</t>
+  </si>
+  <si>
     <t>art001</t>
   </si>
   <si>
@@ -230,6 +315,36 @@
 ទេសចរណ៍ និងបដិសណ្ឋារកិច្ច</t>
   </si>
   <si>
+    <t>car_soc_0046;
+car_soc_0047;
+car_soc_0048;
+car_soc_0049;
+car_soc_0050;
+car_tec_0001;
+car_soc_0051;
+car_soc_0052;
+car_tec_0026;
+car_soc_0053;
+car_soc_0054;
+car_soc_0055;
+car_soc_0056;</t>
+  </si>
+  <si>
+    <t>ប្រវត្តិវិទូ;
+អ្នកសម្ដែងសិល្បៈ;
+អ្នកនិពន្ធ;
+អ្នកដឹកនាំរឿង;
+វិចិត្រករ;
+ស្ថាបត្យករ;
+មគ្គទេសក៍ទេសចរណ៍;
+សាស្ត្រាចារ្យ;
+សេដ្ឋវិទូ;
+បណ្ណាធិការ;
+អ្នករចនាម៉ូដ;
+អ្នកចម្រៀង;
+គ្រូបង្ហាត់ផ្នែករបាំ-ដូរ្យតន្ដ្រី;</t>
+  </si>
+  <si>
     <t>soc001</t>
   </si>
   <si>
@@ -245,7 +360,25 @@
     <t>per_maj_112;
 per_maj_101;
 per_maj_041;
-per_maj_042;</t>
+per_maj_042;
+per_maj_005;
+per_maj_109;
+per_maj_040;
+per_maj_116;
+per_maj_006;
+per_maj_117;
+per_maj_118;
+per_maj_119;
+per_maj_120;
+per_maj_121;
+per_maj_011;
+per_maj_009;
+per_maj_012;
+per_maj_122;
+per_maj_039;
+per_maj_038;
+per_maj_044;
+per_maj_043;</t>
   </si>
   <si>
     <t>ទេសចរណ៍ និងបដិសណ្ឋារកិច្ច;
@@ -272,6 +405,38 @@
 វិទ្យាសាស្ត្រនយោបាយ;</t>
   </si>
   <si>
+    <t>car_soc_0052;
+car_tec_0026;
+car_soc_0024;
+car_soc_0051;
+car_soc_0057;
+car_soc_0058;
+car_soc_0059;
+car_soc_0060;
+car_soc_0053;
+car_soc_0061;
+car_soc_0062;
+car_sci_0028;
+car_soc_0063;
+car_soc_0064</t>
+  </si>
+  <si>
+    <t>សាស្ត្រាចារ្យ;
+សេដ្ឋវិទូ;
+អ្នកសារព័ត៌មាន;
+មគ្គទេសក៍ទេសចរណ៍;
+នាយក-នាយិកាគ្រឹះស្ថានសិក្សា;
+អ្នកនយោបាយ;
+អ្នកគាំពារសង្គម;
+អ្នកផ្ដល់ប្រឹក្សា;
+បណ្ណាធិការ;
+អ្នកបម្រើសេវាសង្គម;
+ឧទ្យានុរក្ស;
+គិលានុបដ្ឋាកយិកា;
+ឱសថការី;
+អ្នកស្រាវជ្រាវ និងអភិវឌ្ឍន៍សង្គម</t>
+  </si>
+  <si>
     <t>ent001</t>
   </si>
   <si>
@@ -288,6 +453,90 @@
 ធ្វើការងារជាលក្ខណៈអ្នកដឹកនាំក្រុម</t>
   </si>
   <si>
+    <t>per_maj_050;
+per_maj_112;
+per_maj_102;
+per_maj_043;
+per_maj_123;
+per_maj_040;
+per_maj_124;
+per_maj_125;
+per_maj_039;
+per_maj_042;
+per_maj_041;
+per_maj_101;
+per_maj_076;
+per_maj_126;
+per_maj_034;
+per_maj_036;
+per_maj_088;
+per_maj_023;
+per_maj_013;
+per_maj_075;
+per_maj_128;</t>
+  </si>
+  <si>
+    <t>បុរាណវិទ្យា;
+ទេសចរណ៍ និងបដិសណ្ឋារកិច្ច;
+សិក្សាអន្ដរជាតិ;
+វិទ្យាសាស្ត្រនយោបាយ;
+ភូមិវិទ្យា;
+ចិត្តវិទ្យា;
+គ្រប់គ្រងពាណិជ្ជកម្ម;
+ស្ថាបត្យកម្ម;
+រដ្ឋបាលសាធារណៈ;
+សង្គមកិច្ចវិទ្យា;
+សង្គមវិទ្យា;
+សេដ្ឋកិច្ច;
+គណនេយ្យ;
+សេដ្ឋកិច្ចអភិវឌ្ឍន៍;
+សេដ្ឋកិច្ចកសិកម្ម និងអភិវឌ្ឍន៍ជនបទ;
+រៀបចំដែនដី និងរដ្ឋបាលដីធ្លី;
+ទូរគមនាគមន៍ និងបណ្ដាញ;
+អភិវឌ្ឍន៍សហគមន៍;
+បរិស្ថាន;
+សហគ្រិនភាព;
+សាសនវិទ្យា;</t>
+  </si>
+  <si>
+    <t>car_soc_0038;
+car_soc_0051;
+car_soc_0058;
+car_soc_0065;
+car_tec_0001;
+car_tec_0026;
+car_soc_0064;
+car_soc_0066;
+car_soc_0067;
+car_soc_0068;
+car_soc_0069;
+car_soc_0070;
+car_tec_0022;
+car_soc_0041;
+car_soc_0042;
+car_soc_0071;
+car_soc_0072;</t>
+  </si>
+  <si>
+    <t>បុរាណវិទូ;
+មគ្គទេសក៍ទេសចរណ៍;
+អ្នកនយោបាយ;
+អ្នកគ្រប់គ្រងអង្គភាព;
+ស្ថាបត្យករ;
+សេដ្ឋវិទូ;
+អ្នកស្រាវជ្រាវ និងអភិវឌ្ឍន៍សង្គម;
+អ្នកជំនាញរៀបចំដែនដី និងរដ្ឋបាលដីធ្លី;
+អ្នកជំនាញផ្នែកបរិស្ថាន;
+សហគ្រិនភាព;
+អ្នកជំនាញខាងសាសនា;
+អ្នកបម្រើសេវាអតិថិជន;
+គណនេយ្យករ;
+មេធាវី;
+ចៅក្រម;
+អ្នកគ្រប់គ្រងផ្នែកអប់រំ និងបណ្ដុះបណ្ដាល;
+អ្នកជំនាញផ្នែកទំនាក់ទំនងសាធារណៈ;</t>
+  </si>
+  <si>
     <t>con001</t>
   </si>
   <si>
@@ -302,6 +551,88 @@
 ធ្វើការងារជាលក្ខណៈមានគណនេយ្យភាព;
 ធ្វើការងារជាលក្ខណៈសមូហភាពគ្រប់គ្រង;
 ធ្វើការងារជាលក្ខណៈគោរពបទបញ្ជា ឬវិន័យខ្ជាប់ខ្ជួន</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per_maj_100;
+per_maj_129;
+per_maj_077;
+per_maj_130;
+per_maj_131;
+per_maj_039;
+per_maj_132;
+per_maj_133;
+per_maj_032;
+per_maj_037;
+per_maj_134;
+per_maj_135;
+per_maj_136;
+per_maj_030;
+per_maj_028;
+per_maj_048;
+per_maj_137;
+per_maj_138;
+per_maj_139;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">វិទ្យាសាស្ត្រកុំព្យូទ័រ;
+គណនេយ្យ និងហិរញ្ញវត្ថុ;
+ធនាគារ និងហិរញ្ញវត្ថុ;
+បច្ចេកវិទ្យា និងនវានុវត្តន៍;
+ប្លង់ និងរចនា;
+រដ្ឋបាលសាធារណៈ;
+គិលានុបដ្ឋាក;
+ឆ្មប;
+វិទ្យាសាស្ត្រជលផល;
+វិទ្យាសាស្ត្រកៅស៊ូ;
+កសិ-ឧស្សាហកម្ម;
+អាហារូបត្ថម្ភ និងសុខភាព;
+កែច្នៃម្ហូបអាហារ;
+វេជ្ជសាស្ត្រសត្វ;
+ក្សេត្រសាស្ត្រ;
+ឱសថសាស្ត្រ;
+វិទ្យាសាស្ត្រទន្ដវទនសាស្ត្រ;
+វិទ្យាសាស្ត្រវេជ្ជសាស្ត្រ;
+វេជ្ជបណ្ឌិតឯកទេស;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car_sci_0045;
+car_sci_0046;
+car_sci_0047;
+car_sci_0029;
+car_sci_0048;
+car_sci_0049;
+car_tec_0015;
+car_sci_0050;
+car_sci_0010;
+car_sci_0008;
+car_tec_0020;
+car_tec_0021;
+car_sci_0051;
+car_sci_0043;
+car_sci_0028;
+car_sci_0052;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ស្មៀន;
+អ្នកជំនាញផ្នែករដ្ឋបាល;
+អ្នកបច្ចេកទេសកុំព្យូទ័រ;
+ឆ្មប;
+អ្នកបច្ចេកទេសជលផល;
+អ្នកបច្ចេកទេសកសិ-ឧស្សាហកម្ម;
+ពេទ្យសត្វ;
+វេជ្ជបណ្ឌិតជំនាញ;
+ទន្ដពេទ្យ;
+អ្នកបច្ចេកទេសកសិកម្ម;
+អ្នកវិភាគហិរញ្ញវត្ថុ;
+សវនករ;
+មន្ត្រីពន្ធដារ;
+អ្នកបច្ចេកទេសខាងចំណីអាហារ;
+គិលានុបដ្ឋាយិកា;
+អ្នករចនាប្លង់;
+</t>
   </si>
 </sst>
 </file>
@@ -409,7 +740,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="41.29"/>
-    <col customWidth="1" min="6" max="7" width="25.57"/>
+    <col customWidth="1" min="5" max="5" width="8.86"/>
+    <col customWidth="1" min="6" max="6" width="12.57"/>
+    <col customWidth="1" min="7" max="7" width="26.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -437,33 +770,38 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -482,31 +820,36 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -525,31 +868,36 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -568,31 +916,36 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -611,27 +964,36 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -650,27 +1012,36 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -689,6 +1060,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>

</xml_diff>